<commit_message>
fix missing SPI2 on TFT_SPI
</commit_message>
<xml_diff>
--- a/EggClassifier.xlsx
+++ b/EggClassifier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c4d86c0fdc6d920/Documents/KiCad/9.0/projects/EggClassifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="11_F25DC773A252ABDACC104818299D70525BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FFE018A-1F0C-421B-8C3B-83FEAF9F29BF}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="11_F25DC773A252ABDACC104818299D70525BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F61E769F-D936-45BD-AC8E-323494BB3D3C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3252" yWindow="2160" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
   <si>
     <t>PA4</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>PG11</t>
+  </si>
+  <si>
+    <t>PG13</t>
   </si>
 </sst>
 </file>
@@ -326,6 +329,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F7:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,7 +852,7 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L18" t="s">
         <v>12</v>
@@ -1175,6 +1182,9 @@
       <c r="M36">
         <v>10</v>
       </c>
+      <c r="N36" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="37" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
@@ -1195,6 +1205,9 @@
       <c r="M37">
         <v>9</v>
       </c>
+      <c r="N37" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="38" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
@@ -1215,6 +1228,9 @@
       <c r="M38">
         <v>12</v>
       </c>
+      <c r="N38" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="39" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
@@ -1235,6 +1251,9 @@
       <c r="M39">
         <v>7</v>
       </c>
+      <c r="N39" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="41" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
@@ -1249,6 +1268,15 @@
       <c r="K41" t="s">
         <v>63</v>
       </c>
+      <c r="L41" t="s">
+        <v>63</v>
+      </c>
+      <c r="O41">
+        <v>13</v>
+      </c>
+      <c r="P41" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="42" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F42" t="s">
@@ -1263,6 +1291,15 @@
       <c r="K42" t="s">
         <v>43</v>
       </c>
+      <c r="L42" t="s">
+        <v>43</v>
+      </c>
+      <c r="O42">
+        <v>16</v>
+      </c>
+      <c r="P42" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
@@ -1277,6 +1314,15 @@
       <c r="I43" t="s">
         <v>11</v>
       </c>
+      <c r="L43" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43">
+        <v>46</v>
+      </c>
+      <c r="N43" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="45" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
@@ -1291,6 +1337,9 @@
       <c r="K45" t="s">
         <v>70</v>
       </c>
+      <c r="L45" t="s">
+        <v>70</v>
+      </c>
       <c r="O45">
         <v>9</v>
       </c>
@@ -1311,6 +1360,9 @@
       <c r="K46" t="s">
         <v>71</v>
       </c>
+      <c r="L46" t="s">
+        <v>71</v>
+      </c>
       <c r="O46">
         <v>10</v>
       </c>
@@ -1331,6 +1383,9 @@
       <c r="K48" t="s">
         <v>72</v>
       </c>
+      <c r="L48" t="s">
+        <v>72</v>
+      </c>
       <c r="O48">
         <v>17</v>
       </c>
@@ -1338,7 +1393,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>67</v>
       </c>
@@ -1354,8 +1409,11 @@
       <c r="O49">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
         <v>68</v>
       </c>
@@ -1368,8 +1426,14 @@
       <c r="K51" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="52" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O51">
+        <v>11</v>
+      </c>
+      <c r="P51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>69</v>
       </c>
@@ -1382,8 +1446,14 @@
       <c r="K52" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O52">
+        <v>12</v>
+      </c>
+      <c r="P52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>70</v>
       </c>
@@ -1396,8 +1466,14 @@
       <c r="K54" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="55" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O54">
+        <v>24</v>
+      </c>
+      <c r="P54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>76</v>
       </c>
@@ -1410,8 +1486,14 @@
       <c r="K55" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O55">
+        <v>28</v>
+      </c>
+      <c r="P55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>48</v>
       </c>
@@ -1424,8 +1506,14 @@
       <c r="K56" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O56">
+        <v>25</v>
+      </c>
+      <c r="P56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>49</v>
       </c>
@@ -1436,6 +1524,12 @@
         <v>34</v>
       </c>
       <c r="K57" t="s">
+        <v>80</v>
+      </c>
+      <c r="O57">
+        <v>18</v>
+      </c>
+      <c r="P57" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>